<commit_message>
se agrego funcion de excel
</commit_message>
<xml_diff>
--- a/uploads/productos.xlsx
+++ b/uploads/productos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>15 ml</t>
   </si>
@@ -70,19 +70,7 @@
     <t>35 ml</t>
   </si>
   <si>
-    <t>nuevo 1</t>
-  </si>
-  <si>
-    <t>nuevo 2</t>
-  </si>
-  <si>
-    <t>nuevo 3</t>
-  </si>
-  <si>
-    <t>nuevo 4</t>
-  </si>
-  <si>
-    <t>nuevo 5</t>
+    <t>Gelish</t>
   </si>
 </sst>
 </file>
@@ -427,7 +415,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E6"/>
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +476,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>3213213211</v>
@@ -508,7 +496,7 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <v>3213213212</v>
@@ -528,7 +516,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>3213213213</v>
@@ -548,7 +536,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>3213213214</v>

</xml_diff>